<commit_message>
Added an intro sequence
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Features</t>
   </si>
@@ -491,7 +491,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,6 +541,9 @@
       </c>
       <c r="D3">
         <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updating the documentation, might start trying to figure out how to map out new animals
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>Features</t>
   </si>
@@ -491,7 +491,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,6 +579,9 @@
       <c r="D5">
         <v>1</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -607,6 +610,9 @@
       <c r="D7">
         <v>1</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -621,6 +627,9 @@
       <c r="D8">
         <v>1</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -631,6 +640,9 @@
       </c>
       <c r="D9">
         <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>